<commit_message>
Gjort massa plottar på ripdatat för att skicka till Karin och Rasmus
</commit_message>
<xml_diff>
--- a/Data/Uppskattat antal ripspillningshögar Helags sommar 2018 distance_sampling.xlsx
+++ b/Data/Uppskattat antal ripspillningshögar Helags sommar 2018 distance_sampling.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,37 +360,12 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Label</t>
+          <t>lya</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Estimate</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>se</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>cv</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>lcl</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>ucl</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>df</t>
+          <t>uppskattat_antal_ripspillningshögar</t>
         </is>
       </c>
     </row>
@@ -401,22 +376,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>26291.71997822703</v>
-      </c>
-      <c r="C2">
-        <v>1546.830104167028</v>
-      </c>
-      <c r="D2">
-        <v>0.05883335534715891</v>
-      </c>
-      <c r="E2">
-        <v>23414.36149045246</v>
-      </c>
-      <c r="F2">
-        <v>29522.67306949076</v>
-      </c>
-      <c r="G2">
-        <v>202.4624373091194</v>
+        <v>36724.77560238716</v>
       </c>
     </row>
     <row r="3">
@@ -426,22 +386,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>15728.81325194428</v>
-      </c>
-      <c r="C3">
-        <v>928.7869553467939</v>
-      </c>
-      <c r="D3">
-        <v>0.05905003387537734</v>
-      </c>
-      <c r="E3">
-        <v>14001.20828972881</v>
-      </c>
-      <c r="F3">
-        <v>17669.5868810141</v>
-      </c>
-      <c r="G3">
-        <v>196.8287288833595</v>
+        <v>21970.30615143725</v>
       </c>
     </row>
     <row r="4">
@@ -451,22 +396,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>14180.20478670656</v>
-      </c>
-      <c r="C4">
-        <v>838.1748310140363</v>
-      </c>
-      <c r="D4">
-        <v>0.05910879593218538</v>
-      </c>
-      <c r="E4">
-        <v>12621.13498201922</v>
-      </c>
-      <c r="F4">
-        <v>15931.86413736982</v>
-      </c>
-      <c r="G4">
-        <v>194.6790111644442</v>
+        <v>19807.1803297371</v>
       </c>
     </row>
     <row r="5">
@@ -476,22 +406,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>11285.64566664929</v>
-      </c>
-      <c r="C5">
-        <v>668.8054013723287</v>
-      </c>
-      <c r="D5">
-        <v>0.05926159841689388</v>
-      </c>
-      <c r="E5">
-        <v>10041.54707592812</v>
-      </c>
-      <c r="F5">
-        <v>12683.88199050371</v>
-      </c>
-      <c r="G5">
-        <v>188.0671965703293</v>
+        <v>15764.00497871487</v>
       </c>
     </row>
     <row r="6">
@@ -501,22 +416,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>14319.42138349049</v>
-      </c>
-      <c r="C6">
-        <v>846.3207048795914</v>
-      </c>
-      <c r="D6">
-        <v>0.05910299600899745</v>
-      </c>
-      <c r="E6">
-        <v>12745.20115950897</v>
-      </c>
-      <c r="F6">
-        <v>16088.08101117993</v>
-      </c>
-      <c r="G6">
-        <v>194.9017292386321</v>
+        <v>20001.64072568122</v>
       </c>
     </row>
     <row r="7">
@@ -526,22 +426,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>4351.981008707895</v>
-      </c>
-      <c r="C7">
-        <v>263.037898619149</v>
-      </c>
-      <c r="D7">
-        <v>0.06044095736926137</v>
-      </c>
-      <c r="E7">
-        <v>3861.589123110629</v>
-      </c>
-      <c r="F7">
-        <v>4904.648862512241</v>
-      </c>
-      <c r="G7">
-        <v>120.7394304590216</v>
+        <v>6078.930024471744</v>
       </c>
     </row>
     <row r="8">
@@ -551,22 +436,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>12228.70696661723</v>
-      </c>
-      <c r="C8">
-        <v>723.9873439715291</v>
-      </c>
-      <c r="D8">
-        <v>0.05920391632148191</v>
-      </c>
-      <c r="E8">
-        <v>10881.99723787608</v>
-      </c>
-      <c r="F8">
-        <v>13742.07976775592</v>
-      </c>
-      <c r="G8">
-        <v>190.7219876932733</v>
+        <v>17081.29097785449</v>
       </c>
     </row>
     <row r="9">
@@ -576,22 +446,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>12646.78241846739</v>
-      </c>
-      <c r="C9">
-        <v>748.450261158574</v>
-      </c>
-      <c r="D9">
-        <v>0.05918108151095049</v>
-      </c>
-      <c r="E9">
-        <v>11254.5806276628</v>
-      </c>
-      <c r="F9">
-        <v>14211.20082848171</v>
-      </c>
-      <c r="G9">
-        <v>191.7220386930659</v>
+        <v>17665.26673778114</v>
       </c>
     </row>
     <row r="10">
@@ -601,22 +456,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>6114.353483308613</v>
-      </c>
-      <c r="C10">
-        <v>366.1920197101401</v>
-      </c>
-      <c r="D10">
-        <v>0.05989055436683478</v>
-      </c>
-      <c r="E10">
-        <v>5432.619190997219</v>
-      </c>
-      <c r="F10">
-        <v>6881.637973226993</v>
-      </c>
-      <c r="G10">
-        <v>152.2956623769574</v>
+        <v>8540.645488927245</v>
       </c>
     </row>
     <row r="11">
@@ -626,47 +466,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>8560.094876632058</v>
-      </c>
-      <c r="C11">
-        <v>509.3184552280023</v>
-      </c>
-      <c r="D11">
-        <v>0.05949916006402864</v>
-      </c>
-      <c r="E11">
-        <v>7612.483269768261</v>
-      </c>
-      <c r="F11">
-        <v>9625.666382472462</v>
-      </c>
-      <c r="G11">
-        <v>175.5837187890006</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B12">
-        <v>125707.7238207508</v>
-      </c>
-      <c r="C12">
-        <v>7363.601666350063</v>
-      </c>
-      <c r="D12">
-        <v>0.05857716170925162</v>
-      </c>
-      <c r="E12">
-        <v>112007.2803780873</v>
-      </c>
-      <c r="F12">
-        <v>141083.9703888185</v>
-      </c>
-      <c r="G12">
-        <v>203.91750427765</v>
+        <v>11956.90368449814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>